<commit_message>
Remove redundant COROS hierarchy
</commit_message>
<xml_diff>
--- a/data/gp3s-devices.xlsx
+++ b/data/gp3s-devices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\gp3s-query\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DBC9CD-4DD1-4BAE-B34D-3596F9D40563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1470E2-C91D-4A3A-A50A-ADD644B85F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CB867C2-8EB5-4F35-9DD0-5D686A7A8D37}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="429">
   <si>
     <t>Amaryllo Trip Tracker</t>
   </si>
@@ -1713,8 +1713,8 @@
   <dimension ref="A1:F249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D186" sqref="D186"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,9 +1827,6 @@
       <c r="C7" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1841,9 +1838,6 @@
       <c r="C8" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1855,9 +1849,6 @@
       <c r="C9" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>391</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1869,9 +1860,6 @@
       <c r="C10" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>392</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1883,9 +1871,6 @@
       <c r="C11" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>393</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1897,9 +1882,6 @@
       <c r="C12" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>394</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1911,9 +1893,6 @@
       <c r="C13" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>394</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1925,9 +1904,6 @@
       <c r="C14" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>395</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1939,9 +1915,6 @@
       <c r="C15" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>395</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1951,9 +1924,6 @@
         <v>241</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="D16" s="1" t="s">
         <v>396</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rethink use of watch series
</commit_message>
<xml_diff>
--- a/data/gp3s-devices.xlsx
+++ b/data/gp3s-devices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\gp3s-query\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1470E2-C91D-4A3A-A50A-ADD644B85F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC4EC60-1826-4945-BF36-453CAF1A4712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CB867C2-8EB5-4F35-9DD0-5D686A7A8D37}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="429">
   <si>
     <t>Amaryllo Trip Tracker</t>
   </si>
@@ -1380,7 +1380,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1714,7 +1722,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,11 +1762,8 @@
       <c r="B2" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>387</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1771,7 +1776,7 @@
       <c r="C3" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>343</v>
       </c>
     </row>
@@ -1785,7 +1790,7 @@
       <c r="C4" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>388</v>
       </c>
     </row>
@@ -1799,7 +1804,7 @@
       <c r="C5" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>388</v>
       </c>
     </row>
@@ -1813,7 +1818,7 @@
       <c r="C6" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -1824,7 +1829,7 @@
       <c r="B7" t="s">
         <v>241</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>389</v>
       </c>
     </row>
@@ -1835,7 +1840,7 @@
       <c r="B8" t="s">
         <v>241</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>390</v>
       </c>
     </row>
@@ -1846,7 +1851,7 @@
       <c r="B9" t="s">
         <v>241</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>391</v>
       </c>
     </row>
@@ -1857,7 +1862,7 @@
       <c r="B10" t="s">
         <v>241</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>392</v>
       </c>
     </row>
@@ -1868,7 +1873,7 @@
       <c r="B11" t="s">
         <v>241</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>393</v>
       </c>
     </row>
@@ -1879,7 +1884,7 @@
       <c r="B12" t="s">
         <v>241</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>394</v>
       </c>
     </row>
@@ -1890,7 +1895,7 @@
       <c r="B13" t="s">
         <v>241</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>394</v>
       </c>
     </row>
@@ -1901,7 +1906,7 @@
       <c r="B14" t="s">
         <v>241</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>395</v>
       </c>
     </row>
@@ -1912,7 +1917,7 @@
       <c r="B15" t="s">
         <v>241</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="3" t="s">
         <v>395</v>
       </c>
     </row>
@@ -1923,7 +1928,7 @@
       <c r="B16" t="s">
         <v>241</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>396</v>
       </c>
     </row>
@@ -1937,7 +1942,7 @@
       <c r="C17" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -1951,7 +1956,7 @@
       <c r="C18" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -1965,10 +1970,7 @@
       <c r="C19" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2139,9 +2141,7 @@
       <c r="C31" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>252</v>
-      </c>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2153,7 +2153,7 @@
       <c r="C32" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="3" t="s">
         <v>404</v>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       <c r="C33" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="3" t="s">
         <v>293</v>
       </c>
       <c r="E33" t="s">
@@ -2184,7 +2184,7 @@
       <c r="C34" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="3" t="s">
         <v>293</v>
       </c>
       <c r="E34" t="s">
@@ -2201,9 +2201,7 @@
       <c r="C35" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>264</v>
-      </c>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
@@ -2285,9 +2283,7 @@
       <c r="C41" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>265</v>
-      </c>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -2313,7 +2309,7 @@
       <c r="C43" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="3" t="s">
         <v>255</v>
       </c>
       <c r="E43" t="s">
@@ -2330,7 +2326,7 @@
       <c r="C44" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="3" t="s">
         <v>255</v>
       </c>
       <c r="E44" t="s">
@@ -2347,7 +2343,7 @@
       <c r="C45" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="3" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2361,7 +2357,7 @@
       <c r="C46" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="3" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2375,7 +2371,7 @@
       <c r="C47" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="3" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2389,7 +2385,7 @@
       <c r="C48" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="3" t="s">
         <v>253</v>
       </c>
       <c r="E48" t="s">
@@ -2406,7 +2402,7 @@
       <c r="C49" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="3" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2420,7 +2416,7 @@
       <c r="C50" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="3" t="s">
         <v>253</v>
       </c>
       <c r="E50" t="s">
@@ -2437,7 +2433,7 @@
       <c r="C51" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="3" t="s">
         <v>253</v>
       </c>
       <c r="E51" t="s">
@@ -2454,7 +2450,7 @@
       <c r="C52" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="3" t="s">
         <v>253</v>
       </c>
       <c r="E52" t="s">
@@ -2471,7 +2467,7 @@
       <c r="C53" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="3" t="s">
         <v>253</v>
       </c>
       <c r="E53" t="s">
@@ -2488,7 +2484,7 @@
       <c r="C54" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="3" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2502,7 +2498,7 @@
       <c r="C55" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="3" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2516,7 +2512,7 @@
       <c r="C56" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="3" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2530,7 +2526,7 @@
       <c r="C57" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="3" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2544,7 +2540,7 @@
       <c r="C58" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="3" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2558,7 +2554,7 @@
       <c r="C59" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="3" t="s">
         <v>410</v>
       </c>
       <c r="E59" t="s">
@@ -2575,7 +2571,7 @@
       <c r="C60" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="3" t="s">
         <v>410</v>
       </c>
     </row>
@@ -2589,7 +2585,7 @@
       <c r="C61" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="3" t="s">
         <v>410</v>
       </c>
       <c r="E61" t="s">
@@ -2606,7 +2602,7 @@
       <c r="C62" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="3" t="s">
         <v>410</v>
       </c>
     </row>
@@ -2620,7 +2616,7 @@
       <c r="C63" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="3" t="s">
         <v>297</v>
       </c>
     </row>
@@ -2634,7 +2630,7 @@
       <c r="C64" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="3" t="s">
         <v>297</v>
       </c>
     </row>
@@ -2648,7 +2644,7 @@
       <c r="C65" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="3" t="s">
         <v>256</v>
       </c>
     </row>
@@ -2662,7 +2658,7 @@
       <c r="C66" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="3" t="s">
         <v>256</v>
       </c>
     </row>
@@ -2676,7 +2672,7 @@
       <c r="C67" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="3" t="s">
         <v>256</v>
       </c>
     </row>
@@ -2690,7 +2686,7 @@
       <c r="C68" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="3" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2704,7 +2700,7 @@
       <c r="C69" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" s="3" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2718,7 +2714,7 @@
       <c r="C70" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E70" t="s">
@@ -2735,7 +2731,7 @@
       <c r="C71" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E71" t="s">
@@ -2752,7 +2748,7 @@
       <c r="C72" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E72" t="s">
@@ -2769,7 +2765,7 @@
       <c r="C73" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E73" t="s">
@@ -2786,7 +2782,7 @@
       <c r="C74" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E74" t="s">
@@ -2803,7 +2799,7 @@
       <c r="C75" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E75" t="s">
@@ -2820,7 +2816,7 @@
       <c r="C76" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E76" t="s">
@@ -2837,7 +2833,7 @@
       <c r="C77" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="3" t="s">
         <v>257</v>
       </c>
     </row>
@@ -2851,7 +2847,7 @@
       <c r="C78" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" s="3" t="s">
         <v>257</v>
       </c>
     </row>
@@ -2865,7 +2861,7 @@
       <c r="C79" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" s="3" t="s">
         <v>257</v>
       </c>
     </row>
@@ -2879,7 +2875,7 @@
       <c r="C80" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" s="3" t="s">
         <v>299</v>
       </c>
       <c r="E80" t="s">
@@ -2896,7 +2892,7 @@
       <c r="C81" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" s="3" t="s">
         <v>299</v>
       </c>
     </row>
@@ -2910,7 +2906,7 @@
       <c r="C82" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" s="3" t="s">
         <v>300</v>
       </c>
     </row>
@@ -2924,7 +2920,7 @@
       <c r="C83" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" s="3" t="s">
         <v>300</v>
       </c>
       <c r="E83" t="s">
@@ -2941,7 +2937,7 @@
       <c r="C84" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" s="3" t="s">
         <v>300</v>
       </c>
       <c r="E84" t="s">
@@ -2958,7 +2954,7 @@
       <c r="C85" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" s="3" t="s">
         <v>300</v>
       </c>
       <c r="E85" t="s">
@@ -2975,7 +2971,7 @@
       <c r="C86" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" s="3" t="s">
         <v>300</v>
       </c>
     </row>
@@ -2989,7 +2985,7 @@
       <c r="C87" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" s="3" t="s">
         <v>258</v>
       </c>
       <c r="E87" t="s">
@@ -3006,7 +3002,7 @@
       <c r="C88" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" s="3" t="s">
         <v>258</v>
       </c>
       <c r="E88" t="s">
@@ -3023,7 +3019,7 @@
       <c r="C89" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" s="3" t="s">
         <v>258</v>
       </c>
       <c r="E89" t="s">
@@ -3040,7 +3036,7 @@
       <c r="C90" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" s="3" t="s">
         <v>258</v>
       </c>
       <c r="E90" t="s">
@@ -3057,7 +3053,7 @@
       <c r="C91" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" s="3" t="s">
         <v>258</v>
       </c>
       <c r="E91" t="s">
@@ -3074,7 +3070,7 @@
       <c r="C92" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" s="3" t="s">
         <v>258</v>
       </c>
       <c r="E92" t="s">
@@ -3091,7 +3087,7 @@
       <c r="C93" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" s="3" t="s">
         <v>258</v>
       </c>
       <c r="E93" t="s">
@@ -3108,7 +3104,7 @@
       <c r="C94" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" s="3" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3122,7 +3118,7 @@
       <c r="C95" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" s="3" t="s">
         <v>301</v>
       </c>
       <c r="E95" t="s">
@@ -3139,7 +3135,7 @@
       <c r="C96" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" s="3" t="s">
         <v>301</v>
       </c>
       <c r="E96" t="s">
@@ -3156,7 +3152,7 @@
       <c r="C97" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" s="3" t="s">
         <v>301</v>
       </c>
       <c r="E97" t="s">
@@ -3173,7 +3169,7 @@
       <c r="C98" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" s="3" t="s">
         <v>301</v>
       </c>
     </row>
@@ -3187,7 +3183,7 @@
       <c r="C99" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" s="3" t="s">
         <v>301</v>
       </c>
       <c r="E99" t="s">
@@ -3204,7 +3200,7 @@
       <c r="C100" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" s="3" t="s">
         <v>301</v>
       </c>
     </row>
@@ -3218,7 +3214,7 @@
       <c r="C101" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" s="3" t="s">
         <v>302</v>
       </c>
       <c r="E101" t="s">
@@ -3235,7 +3231,7 @@
       <c r="C102" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" s="3" t="s">
         <v>302</v>
       </c>
       <c r="E102" t="s">
@@ -3252,7 +3248,7 @@
       <c r="C103" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" s="3" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3266,7 +3262,7 @@
       <c r="C104" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E104" t="s">
@@ -3283,7 +3279,7 @@
       <c r="C105" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E105" t="s">
@@ -3300,7 +3296,7 @@
       <c r="C106" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E106" t="s">
@@ -3317,7 +3313,7 @@
       <c r="C107" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E107" t="s">
@@ -3334,7 +3330,7 @@
       <c r="C108" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E108" t="s">
@@ -3351,7 +3347,7 @@
       <c r="C109" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D109" s="3" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3421,7 +3417,7 @@
       <c r="C114" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" s="3" t="s">
         <v>415</v>
       </c>
     </row>
@@ -3435,7 +3431,7 @@
       <c r="C115" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" s="3" t="s">
         <v>415</v>
       </c>
     </row>
@@ -3449,7 +3445,7 @@
       <c r="C116" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" s="3" t="s">
         <v>312</v>
       </c>
       <c r="E116" t="s">
@@ -3466,7 +3462,7 @@
       <c r="C117" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" s="3" t="s">
         <v>312</v>
       </c>
       <c r="E117" t="s">
@@ -3483,7 +3479,7 @@
       <c r="C118" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D118" s="3" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3497,7 +3493,7 @@
       <c r="C119" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D119" s="3" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3511,7 +3507,7 @@
       <c r="C120" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" s="3" t="s">
         <v>313</v>
       </c>
       <c r="E120" t="s">
@@ -3528,7 +3524,7 @@
       <c r="C121" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D121" s="3" t="s">
         <v>313</v>
       </c>
       <c r="E121" t="s">
@@ -3545,7 +3541,7 @@
       <c r="C122" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D122" s="3" t="s">
         <v>313</v>
       </c>
     </row>
@@ -3559,7 +3555,7 @@
       <c r="C123" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D123" s="3" t="s">
         <v>416</v>
       </c>
     </row>
@@ -3573,7 +3569,7 @@
       <c r="C124" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D124" s="3" t="s">
         <v>417</v>
       </c>
     </row>
@@ -3587,7 +3583,7 @@
       <c r="C125" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D125" s="3" t="s">
         <v>418</v>
       </c>
     </row>
@@ -3601,7 +3597,7 @@
       <c r="C126" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D126" s="3" t="s">
         <v>319</v>
       </c>
     </row>
@@ -3615,7 +3611,7 @@
       <c r="C127" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D127" s="3" t="s">
         <v>319</v>
       </c>
     </row>
@@ -3629,7 +3625,7 @@
       <c r="C128" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D128" s="3" t="s">
         <v>319</v>
       </c>
     </row>
@@ -3643,7 +3639,7 @@
       <c r="C129" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="D129" s="3" t="s">
         <v>419</v>
       </c>
     </row>
@@ -3657,7 +3653,7 @@
       <c r="C130" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D130" s="3" t="s">
         <v>419</v>
       </c>
     </row>
@@ -3671,7 +3667,7 @@
       <c r="C131" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="D131" s="3" t="s">
         <v>420</v>
       </c>
     </row>
@@ -3685,7 +3681,7 @@
       <c r="C132" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D132" s="3" t="s">
         <v>420</v>
       </c>
     </row>
@@ -3699,7 +3695,7 @@
       <c r="C133" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="D133" s="3" t="s">
         <v>421</v>
       </c>
     </row>
@@ -3713,7 +3709,7 @@
       <c r="C134" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D134" s="3" t="s">
         <v>316</v>
       </c>
       <c r="E134" t="s">
@@ -3730,7 +3726,7 @@
       <c r="C135" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="D135" s="3" t="s">
         <v>316</v>
       </c>
       <c r="E135" t="s">
@@ -3747,7 +3743,7 @@
       <c r="C136" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="D136" s="3" t="s">
         <v>422</v>
       </c>
     </row>
@@ -3761,7 +3757,7 @@
       <c r="C137" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D137" s="3" t="s">
         <v>422</v>
       </c>
     </row>
@@ -3775,7 +3771,7 @@
       <c r="C138" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="D138" s="3" t="s">
         <v>351</v>
       </c>
     </row>
@@ -3789,7 +3785,7 @@
       <c r="C139" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="D139" s="3" t="s">
         <v>351</v>
       </c>
     </row>
@@ -3803,7 +3799,7 @@
       <c r="C140" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="D140" s="3" t="s">
         <v>353</v>
       </c>
     </row>
@@ -3817,7 +3813,7 @@
       <c r="C141" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="D141" s="3" t="s">
         <v>353</v>
       </c>
     </row>
@@ -3831,7 +3827,7 @@
       <c r="C142" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="D142" s="3" t="s">
         <v>320</v>
       </c>
     </row>
@@ -3845,7 +3841,7 @@
       <c r="C143" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="D143" s="3" t="s">
         <v>320</v>
       </c>
     </row>
@@ -3859,7 +3855,7 @@
       <c r="C144" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="D144" s="3" t="s">
         <v>320</v>
       </c>
     </row>
@@ -3873,7 +3869,7 @@
       <c r="C145" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="D145" s="3" t="s">
         <v>354</v>
       </c>
     </row>
@@ -3887,7 +3883,7 @@
       <c r="C146" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="D146" s="3" t="s">
         <v>354</v>
       </c>
     </row>
@@ -3901,7 +3897,7 @@
       <c r="C147" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="D147" s="3" t="s">
         <v>317</v>
       </c>
       <c r="E147" t="s">
@@ -3918,7 +3914,7 @@
       <c r="C148" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D148" s="1" t="s">
+      <c r="D148" s="3" t="s">
         <v>317</v>
       </c>
       <c r="E148" t="s">
@@ -3935,7 +3931,7 @@
       <c r="C149" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="D149" s="3" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3949,7 +3945,7 @@
       <c r="C150" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D150" s="1" t="s">
+      <c r="D150" s="3" t="s">
         <v>355</v>
       </c>
     </row>
@@ -3963,7 +3959,7 @@
       <c r="C151" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D151" s="1" t="s">
+      <c r="D151" s="3" t="s">
         <v>356</v>
       </c>
     </row>
@@ -4033,7 +4029,7 @@
       <c r="C156" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="D156" s="3" t="s">
         <v>361</v>
       </c>
       <c r="E156" t="s">
@@ -4050,7 +4046,7 @@
       <c r="C157" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="D157" s="3" t="s">
         <v>361</v>
       </c>
       <c r="E157" t="s">
@@ -4067,7 +4063,7 @@
       <c r="C158" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="D158" s="3" t="s">
         <v>361</v>
       </c>
       <c r="E158" t="s">
@@ -4084,7 +4080,7 @@
       <c r="C159" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="D159" s="3" t="s">
         <v>361</v>
       </c>
       <c r="E159" t="s">
@@ -4101,7 +4097,7 @@
       <c r="C160" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D160" s="1" t="s">
+      <c r="D160" s="3" t="s">
         <v>361</v>
       </c>
       <c r="E160" t="s">
@@ -4118,7 +4114,7 @@
       <c r="C161" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D161" s="1" t="s">
+      <c r="D161" s="3" t="s">
         <v>361</v>
       </c>
       <c r="E161" t="s">
@@ -4135,7 +4131,7 @@
       <c r="C162" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D162" s="1" t="s">
+      <c r="D162" s="3" t="s">
         <v>361</v>
       </c>
       <c r="E162" t="s">
@@ -4152,7 +4148,7 @@
       <c r="C163" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D163" s="1" t="s">
+      <c r="D163" s="3" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4166,7 +4162,7 @@
       <c r="C164" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D164" s="1" t="s">
+      <c r="D164" s="3" t="s">
         <v>362</v>
       </c>
       <c r="E164" t="s">
@@ -4183,7 +4179,7 @@
       <c r="C165" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D165" s="1" t="s">
+      <c r="D165" s="3" t="s">
         <v>362</v>
       </c>
       <c r="E165" t="s">
@@ -4200,7 +4196,7 @@
       <c r="C166" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D166" s="1" t="s">
+      <c r="D166" s="3" t="s">
         <v>362</v>
       </c>
       <c r="E166" t="s">
@@ -4217,7 +4213,7 @@
       <c r="C167" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D167" s="1" t="s">
+      <c r="D167" s="3" t="s">
         <v>362</v>
       </c>
     </row>
@@ -4231,7 +4227,7 @@
       <c r="C168" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D168" s="1" t="s">
+      <c r="D168" s="3" t="s">
         <v>363</v>
       </c>
       <c r="E168" t="s">
@@ -4248,7 +4244,7 @@
       <c r="C169" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D169" s="1" t="s">
+      <c r="D169" s="3" t="s">
         <v>363</v>
       </c>
       <c r="E169" t="s">
@@ -4265,7 +4261,7 @@
       <c r="C170" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="D170" s="3" t="s">
         <v>363</v>
       </c>
       <c r="E170" t="s">
@@ -4282,7 +4278,7 @@
       <c r="C171" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D171" s="1" t="s">
+      <c r="D171" s="3" t="s">
         <v>363</v>
       </c>
     </row>
@@ -4296,7 +4292,7 @@
       <c r="C172" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D172" s="1" t="s">
+      <c r="D172" s="3" t="s">
         <v>364</v>
       </c>
       <c r="E172" t="s">
@@ -4313,7 +4309,7 @@
       <c r="C173" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D173" s="1" t="s">
+      <c r="D173" s="3" t="s">
         <v>364</v>
       </c>
       <c r="E173" t="s">
@@ -4330,7 +4326,7 @@
       <c r="C174" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D174" s="1" t="s">
+      <c r="D174" s="3" t="s">
         <v>364</v>
       </c>
     </row>
@@ -4386,7 +4382,7 @@
       <c r="C178" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D178" s="1" t="s">
+      <c r="D178" s="3" t="s">
         <v>366</v>
       </c>
     </row>
@@ -4400,7 +4396,7 @@
       <c r="C179" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D179" s="1" t="s">
+      <c r="D179" s="3" t="s">
         <v>366</v>
       </c>
       <c r="E179" t="s">
@@ -4417,7 +4413,7 @@
       <c r="C180" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D180" s="1" t="s">
+      <c r="D180" s="3" t="s">
         <v>366</v>
       </c>
     </row>
@@ -4431,7 +4427,7 @@
       <c r="C181" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D181" s="1" t="s">
+      <c r="D181" s="3" t="s">
         <v>326</v>
       </c>
       <c r="E181" t="s">
@@ -4448,7 +4444,7 @@
       <c r="C182" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="D182" s="3" t="s">
         <v>326</v>
       </c>
     </row>
@@ -4462,7 +4458,7 @@
       <c r="C183" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D183" s="1" t="s">
+      <c r="D183" s="3" t="s">
         <v>326</v>
       </c>
     </row>
@@ -4476,7 +4472,7 @@
       <c r="C184" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D184" s="1" t="s">
+      <c r="D184" s="3" t="s">
         <v>327</v>
       </c>
       <c r="E184" t="s">
@@ -4493,7 +4489,7 @@
       <c r="C185" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D185" s="1" t="s">
+      <c r="D185" s="3" t="s">
         <v>327</v>
       </c>
       <c r="E185" t="s">
@@ -4510,7 +4506,7 @@
       <c r="C186" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D186" s="1" t="s">
+      <c r="D186" s="3" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4524,7 +4520,7 @@
       <c r="C187" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D187" s="1" t="s">
+      <c r="D187" s="3" t="s">
         <v>328</v>
       </c>
       <c r="E187" t="s">
@@ -4558,7 +4554,7 @@
       <c r="C189" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D189" s="1" t="s">
+      <c r="D189" s="3" t="s">
         <v>368</v>
       </c>
     </row>
@@ -4572,7 +4568,7 @@
       <c r="C190" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D190" s="1" t="s">
+      <c r="D190" s="3" t="s">
         <v>369</v>
       </c>
     </row>
@@ -4586,7 +4582,7 @@
       <c r="C191" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D191" s="1" t="s">
+      <c r="D191" s="3" t="s">
         <v>369</v>
       </c>
     </row>
@@ -4600,7 +4596,7 @@
       <c r="C192" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D192" s="1" t="s">
+      <c r="D192" s="3" t="s">
         <v>330</v>
       </c>
       <c r="E192" t="s">
@@ -4617,9 +4613,7 @@
       <c r="C193" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="D193" s="3" t="s">
-        <v>370</v>
-      </c>
+      <c r="D193" s="3"/>
     </row>
     <row r="194" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
@@ -4659,9 +4653,7 @@
       <c r="C196" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D196" s="1" t="s">
-        <v>335</v>
-      </c>
+      <c r="D196" s="3"/>
       <c r="E196" t="s">
         <v>268</v>
       </c>
@@ -4676,9 +4668,7 @@
       <c r="C197" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D197" s="1" t="s">
-        <v>335</v>
-      </c>
+      <c r="D197" s="3"/>
       <c r="E197" t="s">
         <v>268</v>
       </c>
@@ -4693,7 +4683,7 @@
       <c r="C198" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D198" s="1" t="s">
+      <c r="D198" s="3" t="s">
         <v>331</v>
       </c>
       <c r="E198" t="s">
@@ -4710,7 +4700,7 @@
       <c r="C199" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D199" s="1" t="s">
+      <c r="D199" s="3" t="s">
         <v>331</v>
       </c>
       <c r="E199" t="s">
@@ -4727,7 +4717,7 @@
       <c r="C200" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D200" s="1" t="s">
+      <c r="D200" s="3" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4741,7 +4731,7 @@
       <c r="C201" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D201" s="1" t="s">
+      <c r="D201" s="3" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4755,7 +4745,7 @@
       <c r="C202" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D202" s="1" t="s">
+      <c r="D202" s="3" t="s">
         <v>332</v>
       </c>
     </row>
@@ -4769,7 +4759,7 @@
       <c r="C203" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D203" s="1" t="s">
+      <c r="D203" s="3" t="s">
         <v>332</v>
       </c>
     </row>
@@ -4783,7 +4773,7 @@
       <c r="C204" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D204" s="1" t="s">
+      <c r="D204" s="3" t="s">
         <v>333</v>
       </c>
     </row>
@@ -4797,7 +4787,7 @@
       <c r="C205" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D205" s="1" t="s">
+      <c r="D205" s="3" t="s">
         <v>333</v>
       </c>
     </row>
@@ -4811,7 +4801,7 @@
       <c r="C206" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D206" s="1" t="s">
+      <c r="D206" s="3" t="s">
         <v>334</v>
       </c>
     </row>
@@ -4859,7 +4849,7 @@
       <c r="C209" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D209" s="1" t="s">
+      <c r="D209" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -4873,7 +4863,7 @@
       <c r="C210" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D210" s="1" t="s">
+      <c r="D210" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -4884,11 +4874,8 @@
       <c r="B211" t="s">
         <v>339</v>
       </c>
-      <c r="C211" s="1" t="s">
+      <c r="D211" s="3" t="s">
         <v>373</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -4898,11 +4885,8 @@
       <c r="B212" t="s">
         <v>242</v>
       </c>
-      <c r="C212" s="1" t="s">
+      <c r="D212" s="3" t="s">
         <v>374</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -4912,11 +4896,8 @@
       <c r="B213" t="s">
         <v>243</v>
       </c>
-      <c r="C213" s="1" t="s">
+      <c r="D213" s="3" t="s">
         <v>375</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -4926,11 +4907,8 @@
       <c r="B214" t="s">
         <v>243</v>
       </c>
-      <c r="C214" s="1" t="s">
+      <c r="D214" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -4940,11 +4918,8 @@
       <c r="B215" t="s">
         <v>243</v>
       </c>
-      <c r="C215" s="1" t="s">
+      <c r="D215" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="D215" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -4954,11 +4929,8 @@
       <c r="B216" t="s">
         <v>243</v>
       </c>
-      <c r="C216" s="1" t="s">
+      <c r="D216" s="3" t="s">
         <v>377</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -4968,11 +4940,8 @@
       <c r="B217" t="s">
         <v>340</v>
       </c>
-      <c r="C217" s="1" t="s">
+      <c r="D217" s="3" t="s">
         <v>373</v>
-      </c>
-      <c r="D217" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -4985,7 +4954,7 @@
       <c r="C218" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D218" s="1" t="s">
+      <c r="D218" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -4999,7 +4968,7 @@
       <c r="C219" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D219" s="1" t="s">
+      <c r="D219" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5013,7 +4982,7 @@
       <c r="C220" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D220" s="1" t="s">
+      <c r="D220" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5027,7 +4996,7 @@
       <c r="C221" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D221" s="1" t="s">
+      <c r="D221" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5038,10 +5007,7 @@
       <c r="B222" t="s">
         <v>244</v>
       </c>
-      <c r="C222" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D222" s="1" t="s">
+      <c r="D222" s="3" t="s">
         <v>378</v>
       </c>
       <c r="E222" t="s">
@@ -5055,10 +5021,7 @@
       <c r="B223" t="s">
         <v>244</v>
       </c>
-      <c r="C223" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D223" s="1" t="s">
+      <c r="D223" s="3" t="s">
         <v>378</v>
       </c>
     </row>
@@ -5069,10 +5032,7 @@
       <c r="B224" t="s">
         <v>244</v>
       </c>
-      <c r="C224" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="D224" s="1" t="s">
+      <c r="D224" s="3" t="s">
         <v>379</v>
       </c>
     </row>
@@ -5083,10 +5043,7 @@
       <c r="B225" t="s">
         <v>244</v>
       </c>
-      <c r="C225" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D225" s="1" t="s">
+      <c r="D225" s="3" t="s">
         <v>380</v>
       </c>
       <c r="E225" t="s">
@@ -5100,10 +5057,7 @@
       <c r="B226" t="s">
         <v>244</v>
       </c>
-      <c r="C226" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D226" s="1" t="s">
+      <c r="D226" s="3" t="s">
         <v>380</v>
       </c>
       <c r="E226" t="s">
@@ -5117,10 +5071,7 @@
       <c r="B227" t="s">
         <v>244</v>
       </c>
-      <c r="C227" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D227" s="1" t="s">
+      <c r="D227" s="3" t="s">
         <v>380</v>
       </c>
     </row>
@@ -5134,7 +5085,7 @@
       <c r="C228" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D228" s="1" t="s">
+      <c r="D228" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5148,9 +5099,7 @@
       <c r="C229" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D229" s="1" t="s">
-        <v>381</v>
-      </c>
+      <c r="D229" s="3"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
@@ -5162,9 +5111,7 @@
       <c r="C230" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D230" s="1" t="s">
-        <v>381</v>
-      </c>
+      <c r="D230" s="3"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
@@ -5176,7 +5123,7 @@
       <c r="C231" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D231" s="1" t="s">
+      <c r="D231" s="3" t="s">
         <v>382</v>
       </c>
       <c r="E231" t="s">
@@ -5193,7 +5140,7 @@
       <c r="C232" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D232" s="1" t="s">
+      <c r="D232" s="3" t="s">
         <v>382</v>
       </c>
       <c r="E232" t="s">
@@ -5210,7 +5157,7 @@
       <c r="C233" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D233" s="1" t="s">
+      <c r="D233" s="3" t="s">
         <v>382</v>
       </c>
     </row>
@@ -5224,7 +5171,7 @@
       <c r="C234" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D234" s="1" t="s">
+      <c r="D234" s="3" t="s">
         <v>286</v>
       </c>
       <c r="E234" t="s">
@@ -5241,7 +5188,7 @@
       <c r="C235" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D235" s="1" t="s">
+      <c r="D235" s="3" t="s">
         <v>286</v>
       </c>
       <c r="E235" t="s">
@@ -5258,7 +5205,7 @@
       <c r="C236" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D236" s="1" t="s">
+      <c r="D236" s="3" t="s">
         <v>286</v>
       </c>
       <c r="E236" t="s">
@@ -5272,11 +5219,9 @@
       <c r="B237" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C237" s="3" t="s">
+      <c r="C237" s="3"/>
+      <c r="D237" s="3" t="s">
         <v>383</v>
-      </c>
-      <c r="D237" s="3" t="s">
-        <v>372</v>
       </c>
       <c r="F237" s="2" t="s">
         <v>347</v>
@@ -5289,11 +5234,9 @@
       <c r="B238" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C238" s="3" t="s">
+      <c r="C238" s="3"/>
+      <c r="D238" s="3" t="s">
         <v>384</v>
-      </c>
-      <c r="D238" s="3" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
@@ -5306,7 +5249,7 @@
       <c r="C239" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D239" s="1" t="s">
+      <c r="D239" s="3" t="s">
         <v>385</v>
       </c>
       <c r="E239" t="s">
@@ -5323,7 +5266,7 @@
       <c r="C240" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D240" s="1" t="s">
+      <c r="D240" s="3" t="s">
         <v>385</v>
       </c>
     </row>
@@ -5337,7 +5280,7 @@
       <c r="C241" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D241" s="1" t="s">
+      <c r="D241" s="3" t="s">
         <v>341</v>
       </c>
       <c r="E241" t="s">
@@ -5354,7 +5297,7 @@
       <c r="C242" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D242" s="1" t="s">
+      <c r="D242" s="3" t="s">
         <v>386</v>
       </c>
     </row>
@@ -5365,9 +5308,7 @@
       <c r="B243" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C243" s="3" t="s">
-        <v>290</v>
-      </c>
+      <c r="C243" s="3"/>
       <c r="D243" s="3" t="s">
         <v>290</v>
       </c>
@@ -5385,7 +5326,7 @@
       <c r="C244" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D244" s="1" t="s">
+      <c r="D244" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5399,7 +5340,7 @@
       <c r="C245" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D245" s="1" t="s">
+      <c r="D245" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5413,7 +5354,7 @@
       <c r="C246" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D246" s="1" t="s">
+      <c r="D246" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5427,7 +5368,7 @@
       <c r="C247" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D247" s="1" t="s">
+      <c r="D247" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5438,11 +5379,8 @@
       <c r="B248" t="s">
         <v>245</v>
       </c>
-      <c r="C248" s="1" t="s">
+      <c r="D248" s="3" t="s">
         <v>373</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -5452,11 +5390,8 @@
       <c r="B249" t="s">
         <v>245</v>
       </c>
-      <c r="C249" s="1" t="s">
+      <c r="D249" s="3" t="s">
         <v>373</v>
-      </c>
-      <c r="D249" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>